<commit_message>
Finished code explanation(will add more later)
</commit_message>
<xml_diff>
--- a/Visual Code Explanation.xlsx
+++ b/Visual Code Explanation.xlsx
@@ -1344,7 +1344,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Misc. functions</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1398,7 +1401,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Misc. functions</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1452,6 +1458,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Misc.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> functions</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -1506,7 +1520,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Misc. functions</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1612,14 +1629,14 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1662,14 +1679,14 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1712,14 +1729,14 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1766,14 +1783,14 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -2154,7 +2171,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2165,7 +2182,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1371600" y="533400"/>
-          <a:ext cx="2162175" cy="771525"/>
+          <a:ext cx="2162175" cy="962025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2213,6 +2230,13 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>rectodc=reciever to datacontroller</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>chtodc=commandhandler to datacontroller</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2521,7 +2545,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Misc. functions</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2678,6 +2705,474 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="533400"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>NOTE:will</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> add dctotrm</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>for transmitter</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1171575" y="2447925"/>
+          <a:ext cx="914400" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Datacontroller</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> controls the flow of data throughout the program</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Rectangle 50"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219199" y="4381500"/>
+          <a:ext cx="1076325" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Network sends</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>/recieves</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>data from the server</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Rectangle 51"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9048750" y="4467223"/>
+          <a:ext cx="914400" cy="1657351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>CommandHandler controls the UI and distributes commands to the program from the UI</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Rectangle 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14020800" y="4952999"/>
+          <a:ext cx="914400" cy="1285875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Transmitter</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> controls the output of data to LIS and buffers it accordingly</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Rectangle 53"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13935075" y="2447924"/>
+          <a:ext cx="914400" cy="1152525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Reciever recieves</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> data from LIS and buffers it accordingly</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Curved Connector 15"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="1035" idx="2"/>
+          <a:endCxn id="47" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2971800" y="2914650"/>
+          <a:ext cx="152400" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
         <a:lnRef idx="1">
           <a:schemeClr val="accent1"/>
         </a:lnRef>
@@ -2692,6 +3187,612 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Curved Connector 17"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="47" idx="3"/>
+          <a:endCxn id="50" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3790950" y="3209925"/>
+          <a:ext cx="8382000" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Curved Connector 21"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="47" idx="3"/>
+          <a:endCxn id="48" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3790950" y="3209925"/>
+          <a:ext cx="12700" cy="2457450"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1800000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Curved Connector 23"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="47" idx="3"/>
+          <a:endCxn id="49" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3790950" y="3209925"/>
+          <a:ext cx="8429625" cy="2381250"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Curved Connector 25"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="82" idx="1"/>
+          <a:endCxn id="48" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3790950" y="5667375"/>
+          <a:ext cx="3562350" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Curved Connector 27"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="82" idx="1"/>
+          <a:endCxn id="47" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3790950" y="3209925"/>
+          <a:ext cx="3562350" cy="3219450"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Curved Connector 29"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="44" idx="2"/>
+          <a:endCxn id="48" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2838451" y="5229225"/>
+          <a:ext cx="428625" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Curved Connector 31"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="46" idx="2"/>
+          <a:endCxn id="50" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="12739688" y="2947988"/>
+          <a:ext cx="361950" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Curved Connector 33"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="45" idx="2"/>
+          <a:endCxn id="49" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="12758738" y="5167312"/>
+          <a:ext cx="390525" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466724</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Flowchart: Process 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1685924" y="6438899"/>
+          <a:ext cx="3533775" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>NOTE: if this is hard to understand for some of you just look at the code for detailed</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> comments</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Flowchart: Process 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11210924" y="6562724"/>
+          <a:ext cx="2905125" cy="828675"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartProcess">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>NOTE:this will be updated</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> as the code updates so if this appears slightly different than the actual code it is because i updated what i am about to do or vice/versa</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2962,8 +4063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Touched up on Explanation
</commit_message>
<xml_diff>
--- a/Visual Code Explanation.xlsx
+++ b/Visual Code Explanation.xlsx
@@ -1299,15 +1299,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1316,7 +1316,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2305050" y="2990850"/>
+          <a:off x="2295525" y="3200400"/>
           <a:ext cx="1485900" cy="438150"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -1874,8 +1874,8 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1885,7 +1885,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13611224" y="180974"/>
-          <a:ext cx="1819275" cy="2095501"/>
+          <a:ext cx="1819275" cy="2171701"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -1976,7 +1976,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>200024</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1989,7 +1989,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12392025" y="819150"/>
-          <a:ext cx="1219199" cy="409575"/>
+          <a:ext cx="1219199" cy="447675"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -2116,13 +2116,13 @@
       <xdr:col>25</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>111062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>111062</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2133,9 +2133,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15430499" y="1228725"/>
-          <a:ext cx="533401" cy="25337"/>
+        <a:xfrm flipV="1">
+          <a:off x="15430499" y="1254062"/>
+          <a:ext cx="533401" cy="12763"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -2257,8 +2257,8 @@
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2268,7 +2268,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15668625" y="2724150"/>
-          <a:ext cx="1771650" cy="2457450"/>
+          <a:ext cx="1771650" cy="1181100"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -2831,13 +2831,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2846,8 +2846,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1171575" y="2447925"/>
-          <a:ext cx="914400" cy="1085850"/>
+          <a:off x="1171575" y="2447924"/>
+          <a:ext cx="914400" cy="1133475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3079,15 +3079,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3096,7 +3096,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13935075" y="2447924"/>
+          <a:off x="13973175" y="2457449"/>
           <a:ext cx="914400" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3141,15 +3141,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>603250</xdr:colOff>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3161,8 +3161,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2971800" y="2914650"/>
-          <a:ext cx="152400" cy="12700"/>
+          <a:off x="2862263" y="3014663"/>
+          <a:ext cx="361950" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -3192,15 +3192,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3211,9 +3211,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3790950" y="3209925"/>
-          <a:ext cx="8382000" cy="142875"/>
+        <a:xfrm flipV="1">
+          <a:off x="3781425" y="3352800"/>
+          <a:ext cx="8391525" cy="66675"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -3243,13 +3243,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>146050</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -3263,12 +3263,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3790950" y="3209925"/>
-          <a:ext cx="12700" cy="2457450"/>
+          <a:off x="3781425" y="3419475"/>
+          <a:ext cx="9525" cy="2247900"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 1800000"/>
+            <a:gd name="adj1" fmla="val 2500000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -3296,9 +3296,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
@@ -3316,8 +3316,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3790950" y="3209925"/>
-          <a:ext cx="8429625" cy="2381250"/>
+          <a:off x="3781425" y="3419475"/>
+          <a:ext cx="8439150" cy="2171700"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -3398,13 +3398,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>38101</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -3418,8 +3418,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3790950" y="3209925"/>
-          <a:ext cx="3562350" cy="3219450"/>
+          <a:off x="3781426" y="3419475"/>
+          <a:ext cx="3571875" cy="3009900"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -3793,6 +3793,57 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Curved Connector 16"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="81" idx="2"/>
+          <a:endCxn id="82" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="7934325" y="6048374"/>
+          <a:ext cx="314325" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4063,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>